<commit_message>
fifo doc and vhdl created.
</commit_message>
<xml_diff>
--- a/doc/super-duper-nes-architecture.xlsx
+++ b/doc/super-duper-nes-architecture.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\super-duper-nes\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daisuke\nes\super-duper-nes\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="architecture" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="block diagram" sheetId="2" r:id="rId2"/>
+    <sheet name="memory map" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Fami con cartlidge I/F</t>
   </si>
@@ -45,29 +45,226 @@
   <si>
     <t>IDE 40 pins flat cable I/F</t>
   </si>
+  <si>
+    <t>NES cartridge</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I/F</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I2C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GPIO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>zp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0100</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0200</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0800</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2008</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x4000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x4020</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x6000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x8000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x10000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xc000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mirror</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0000-0x07ff</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>io reg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>io reg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2000-0x2007</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>expantion rom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sram</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>prog rom</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower bank</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>upper bank</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CPU space</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>memory map</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ram</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>duper io reg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reset vector</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fifo status register</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r: pop fifo register</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w: push fifo register</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xfffa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xfff9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xfff8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>firo status register</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>write fifo empty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>write fifo full</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>read fifo empty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>read fifo full</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>always 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -75,15 +272,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -115,7 +395,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -174,7 +460,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -234,7 +526,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -289,7 +587,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -344,7 +648,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -399,7 +709,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -454,7 +770,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectangle 16"/>
+        <xdr:cNvPr id="17" name="Rectangle 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -509,7 +831,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle 17"/>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -564,20 +892,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="33" name="Group 32"/>
+        <xdr:cNvPr id="33" name="Group 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2008909" y="1050858"/>
-          <a:ext cx="277091" cy="473142"/>
+          <a:off x="2320636" y="964267"/>
+          <a:ext cx="346364" cy="421188"/>
           <a:chOff x="2024495" y="1143000"/>
           <a:chExt cx="280555" cy="762000"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="15" name="Group 14"/>
+          <xdr:cNvPr id="15" name="Group 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
@@ -590,7 +930,13 @@
         </xdr:grpSpPr>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="9" name="Straight Connector 8"/>
+            <xdr:cNvPr id="9" name="Straight Connector 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -619,7 +965,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="10" name="Straight Connector 9"/>
+            <xdr:cNvPr id="10" name="Straight Connector 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -648,7 +1000,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="11" name="Straight Connector 10"/>
+            <xdr:cNvPr id="11" name="Straight Connector 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -677,7 +1035,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="12" name="Straight Connector 11"/>
+            <xdr:cNvPr id="12" name="Straight Connector 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -706,7 +1070,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="13" name="Straight Connector 12"/>
+            <xdr:cNvPr id="13" name="Straight Connector 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -735,7 +1105,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="14" name="Straight Connector 13"/>
+            <xdr:cNvPr id="14" name="Straight Connector 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -765,7 +1141,13 @@
       </xdr:grpSp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="26" name="Group 25"/>
+          <xdr:cNvPr id="26" name="Group 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
@@ -778,7 +1160,13 @@
         </xdr:grpSpPr>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="27" name="Straight Connector 26"/>
+            <xdr:cNvPr id="27" name="Straight Connector 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -807,7 +1195,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="28" name="Straight Connector 27"/>
+            <xdr:cNvPr id="28" name="Straight Connector 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -836,7 +1230,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="29" name="Straight Connector 28"/>
+            <xdr:cNvPr id="29" name="Straight Connector 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -865,7 +1265,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="30" name="Straight Connector 29"/>
+            <xdr:cNvPr id="30" name="Straight Connector 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -894,7 +1300,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="31" name="Straight Connector 30"/>
+            <xdr:cNvPr id="31" name="Straight Connector 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -923,7 +1335,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="32" name="Straight Connector 31"/>
+            <xdr:cNvPr id="32" name="Straight Connector 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -969,20 +1387,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="34" name="Group 33"/>
+        <xdr:cNvPr id="34" name="Group 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2008909" y="1570071"/>
-          <a:ext cx="277091" cy="473142"/>
+          <a:off x="2320636" y="1431526"/>
+          <a:ext cx="346364" cy="438505"/>
           <a:chOff x="2024495" y="1143000"/>
           <a:chExt cx="280555" cy="762000"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="35" name="Group 34"/>
+          <xdr:cNvPr id="35" name="Group 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
@@ -995,7 +1425,13 @@
         </xdr:grpSpPr>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="43" name="Straight Connector 42"/>
+            <xdr:cNvPr id="43" name="Straight Connector 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1024,7 +1460,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="44" name="Straight Connector 43"/>
+            <xdr:cNvPr id="44" name="Straight Connector 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1053,7 +1495,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="45" name="Straight Connector 44"/>
+            <xdr:cNvPr id="45" name="Straight Connector 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1082,7 +1530,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="46" name="Straight Connector 45"/>
+            <xdr:cNvPr id="46" name="Straight Connector 45">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1111,7 +1565,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="47" name="Straight Connector 46"/>
+            <xdr:cNvPr id="47" name="Straight Connector 46">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1140,7 +1600,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="48" name="Straight Connector 47"/>
+            <xdr:cNvPr id="48" name="Straight Connector 47">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1170,7 +1636,13 @@
       </xdr:grpSp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="36" name="Group 35"/>
+          <xdr:cNvPr id="36" name="Group 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
@@ -1183,7 +1655,13 @@
         </xdr:grpSpPr>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="37" name="Straight Connector 36"/>
+            <xdr:cNvPr id="37" name="Straight Connector 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1212,7 +1690,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="38" name="Straight Connector 37"/>
+            <xdr:cNvPr id="38" name="Straight Connector 37">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1241,7 +1725,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="39" name="Straight Connector 38"/>
+            <xdr:cNvPr id="39" name="Straight Connector 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1270,7 +1760,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="40" name="Straight Connector 39"/>
+            <xdr:cNvPr id="40" name="Straight Connector 39">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1299,7 +1795,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="41" name="Straight Connector 40"/>
+            <xdr:cNvPr id="41" name="Straight Connector 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1328,7 +1830,13 @@
         </xdr:cxnSp>
         <xdr:cxnSp macro="">
           <xdr:nvCxnSpPr>
-            <xdr:cNvPr id="42" name="Straight Connector 41"/>
+            <xdr:cNvPr id="42" name="Straight Connector 41">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvCxnSpPr/>
           </xdr:nvCxnSpPr>
           <xdr:spPr>
@@ -1374,7 +1882,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Rectangle 48"/>
+        <xdr:cNvPr id="49" name="Rectangle 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1429,7 +1943,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Rounded Rectangle 49"/>
+        <xdr:cNvPr id="50" name="Rounded Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1484,7 +2004,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="Straight Connector 51"/>
+        <xdr:cNvPr id="52" name="Straight Connector 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="2" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -1530,7 +2056,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Rectangle 50"/>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1590,7 +2122,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="Rectangle 52"/>
+        <xdr:cNvPr id="53" name="Rectangle 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1645,20 +2183,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="Group 2"/>
+        <xdr:cNvPr id="3" name="Group 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="5400000" flipV="1">
-          <a:off x="5226593" y="2167891"/>
-          <a:ext cx="571502" cy="45719"/>
+          <a:off x="6153115" y="1968732"/>
+          <a:ext cx="519548" cy="45719"/>
           <a:chOff x="6705600" y="1333500"/>
           <a:chExt cx="1047750" cy="76200"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="55" name="Straight Connector 54"/>
+          <xdr:cNvPr id="55" name="Straight Connector 54">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1687,7 +2237,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="56" name="Straight Connector 55"/>
+          <xdr:cNvPr id="56" name="Straight Connector 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1732,7 +2288,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="Rectangle 60"/>
+        <xdr:cNvPr id="61" name="Rectangle 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1792,20 +2354,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="76" name="Group 75"/>
+        <xdr:cNvPr id="76" name="Group 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3119004" y="1524000"/>
-          <a:ext cx="1538721" cy="952501"/>
+          <a:off x="3603913" y="1385455"/>
+          <a:ext cx="1815812" cy="865910"/>
           <a:chOff x="3160272" y="1524000"/>
           <a:chExt cx="1562304" cy="952501"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="20" name="Straight Connector 19"/>
+          <xdr:cNvPr id="20" name="Straight Connector 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1834,7 +2408,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="21" name="Straight Connector 20"/>
+          <xdr:cNvPr id="21" name="Straight Connector 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1863,7 +2443,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="22" name="Straight Connector 21"/>
+          <xdr:cNvPr id="22" name="Straight Connector 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1892,7 +2478,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="23" name="Straight Connector 22"/>
+          <xdr:cNvPr id="23" name="Straight Connector 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1921,7 +2513,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="24" name="Straight Connector 23"/>
+          <xdr:cNvPr id="24" name="Straight Connector 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1950,7 +2548,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="25" name="Straight Connector 24"/>
+          <xdr:cNvPr id="25" name="Straight Connector 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1979,7 +2583,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="58" name="Straight Connector 57"/>
+          <xdr:cNvPr id="58" name="Straight Connector 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2008,7 +2618,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="59" name="Straight Connector 58"/>
+          <xdr:cNvPr id="59" name="Straight Connector 58">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2037,7 +2653,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="60" name="Straight Connector 59"/>
+          <xdr:cNvPr id="60" name="Straight Connector 59">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2066,7 +2688,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="62" name="Straight Connector 61"/>
+          <xdr:cNvPr id="62" name="Straight Connector 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2095,7 +2723,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="63" name="Straight Connector 62"/>
+          <xdr:cNvPr id="63" name="Straight Connector 62">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2124,7 +2758,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="64" name="Straight Connector 63"/>
+          <xdr:cNvPr id="64" name="Straight Connector 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -2169,7 +2809,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1027" name="AutoShape 3" descr="http://img2.banggood.com/thumb/large/upload/2012/chenjianwei/SKU109915.%284%29.jpg"/>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="http://img2.banggood.com/thumb/large/upload/2012/chenjianwei/SKU109915.%284%29.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2211,7 +2857,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="AutoShape 4" descr="http://img2.banggood.com/thumb/large/upload/2012/chenjianwei/SKU109915.(4).jpg"/>
+        <xdr:cNvPr id="1028" name="AutoShape 4" descr="http://img2.banggood.com/thumb/large/upload/2012/chenjianwei/SKU109915.(4).jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2253,7 +2905,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1029" name="AutoShape 5" descr="http://img2.banggood.com/thumb/large/upload/2012/chenjianwei/SKU109915.(4).jpg"/>
+        <xdr:cNvPr id="1029" name="AutoShape 5" descr="http://img2.banggood.com/thumb/large/upload/2012/chenjianwei/SKU109915.(4).jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2295,7 +2953,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="77" name="Picture 76"/>
+        <xdr:cNvPr id="77" name="Picture 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2322,6 +2986,1489 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2247679-251F-4D88-8F07-EBF546E0DA7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362199" y="1362074"/>
+          <a:ext cx="2657475" cy="2409825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>NES</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7926CF31-A546-41A3-A15E-4DE17B509DFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514599" y="1704975"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>CPU 6502</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FA88FD-76BF-4D56-B4F1-2D57299C29D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514599" y="2733675"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>PPU</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A881FC7-CB09-4132-9927-9B06F74FBAC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3838575" y="1714500"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>RAM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>2k</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FACFA3D8-FD6C-4C3C-9596-F9638F17BCD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4133851" y="1371600"/>
+          <a:ext cx="3543300" cy="2914650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>DE0-CV</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{357D6DFE-DB23-4599-8D0E-C7E8AC62484B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6200775" y="1714500"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>PROM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>32k</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="正方形/長方形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480753E1-924B-401E-83E1-0CBF6C2188C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6200775" y="2733675"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>CROM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>8k</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="正方形/長方形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917DB88B-F309-458C-AD46-850FBC2B7944}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7534275" y="1714500"/>
+          <a:ext cx="733426" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>FIFO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>256</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> byte</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBA1A6A1-6BA6-4AE9-9F42-196036AF39CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7534274" y="2733675"/>
+          <a:ext cx="733426" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>FIFO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>256</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> byte</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="正方形/長方形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFB6A670-37C2-488C-9D57-63BA8A7B60C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8562975" y="2228850"/>
+          <a:ext cx="590550" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>I2C</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Slave</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A65B060D-433B-402F-AFD7-22C6564EEE99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3838575" y="2733675"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>VRAM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>2k</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A178BF2-AD68-4847-AD0B-CA631F33E095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8562974" y="1362075"/>
+          <a:ext cx="4429125" cy="2409825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Beagle bone</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="正方形/長方形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAEEB55E-E5CD-4A51-8DDF-551E4BE83633}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9010649" y="1714500"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>CPU</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>AM3358</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="正方形/長方形 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA4312F7-7630-4D28-AFF7-2E9465A12464}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9010649" y="2733675"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>DDR3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>512MB</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="正方形/長方形 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC88A48A-853C-46DD-84FB-8B63D6F573F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10334625" y="1714500"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>EEPROM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>4k</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="正方形/長方形 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A2A49E-0EDF-4834-BA90-2B39D7E01C4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11668124" y="1714500"/>
+          <a:ext cx="1028701" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>onboard</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> NAND</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t>eMMC 4GB</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="正方形/長方形 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{520241A1-91AC-40D3-AEFC-3B6EDFC9C203}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876799" y="3600451"/>
+          <a:ext cx="1914526" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>GPIO</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="正方形/長方形 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E6C182F-89E5-4134-A625-076B97F1A078}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11372849" y="3086100"/>
+          <a:ext cx="1323976" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>GPIO</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="正方形/長方形 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC6B2AD-7AFB-4F1F-BA4F-D8A81C7D71CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10334625" y="2733675"/>
+          <a:ext cx="590550" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>I2C</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Master</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="直線コネクタ 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0DE781-A5A9-4D1C-98EA-5EA777BB4999}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3248024" y="2566987"/>
+          <a:ext cx="885827" cy="4763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直線コネクタ 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C42186A-D4F8-4097-86DB-3963A51FE7C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3695700" y="2409825"/>
+          <a:ext cx="0" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直線コネクタ 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{990E9ABF-DDA1-496F-A306-1C4028430B36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="13" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7677151" y="2566987"/>
+          <a:ext cx="885823" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直線コネクタ 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0601CF1-55BD-4263-86F9-F8C5122A8EEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8124824" y="2400300"/>
+          <a:ext cx="0" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2589,21 +4736,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="H8:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO14"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="8" spans="11:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="11:28" x14ac:dyDescent="0.15">
       <c r="Q8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="11:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="11:28" x14ac:dyDescent="0.15">
       <c r="K12" t="s">
         <v>0</v>
       </c>
@@ -2611,47 +4758,380 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="11:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="11:28" x14ac:dyDescent="0.15">
       <c r="K13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="11:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="11:28" x14ac:dyDescent="0.15">
       <c r="K14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.15">
       <c r="H22" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="L17:AB18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB19" sqref="AB19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="3.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="17" spans="12:28" x14ac:dyDescent="0.15">
+      <c r="L17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="12:28" x14ac:dyDescent="0.15">
+      <c r="L18" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A3:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="3.875" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C13" s="1"/>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="10">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="F15" s="10">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="F16" s="10">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C17" s="1"/>
+      <c r="D17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="10">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="10">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="10">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C20" s="1"/>
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C26" s="1"/>
+      <c r="D26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C27" s="1"/>
+      <c r="D27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C32" s="1"/>
+      <c r="D32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C33" s="1"/>
+      <c r="D33" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C36" s="1"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modelsim simulation work update.
</commit_message>
<xml_diff>
--- a/doc/super-duper-nes-architecture.xlsx
+++ b/doc/super-duper-nes-architecture.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="architecture" sheetId="1" r:id="rId1"/>
     <sheet name="block diagram" sheetId="2" r:id="rId2"/>
     <sheet name="memory map" sheetId="3" r:id="rId3"/>
+    <sheet name="nes-bbb-if" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -4474,6 +4475,1435 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8955E15-C818-4052-9C19-D8FF9B82FF30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000126" y="857250"/>
+          <a:ext cx="1200150" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>NES</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5713A0F4-827F-4C67-B3DD-F632AD6C7D79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2800350" y="342900"/>
+          <a:ext cx="5400676" cy="4457700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>DE0-CV</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820767D0-A403-4007-A7F1-C06E192A4F8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10001250" y="857250"/>
+          <a:ext cx="1200150" cy="2228850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>BBB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F36E6E7-DA55-4C11-A7E9-796EBC9DA1CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3400426" y="685800"/>
+          <a:ext cx="4400550" cy="2543176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Duper Cartridge</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896D09C2-970F-4850-AE42-A3B5D7CF8E76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3400425" y="3771900"/>
+          <a:ext cx="1400175" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>CHRROM</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2ECDDA-35B8-43FE-8CDC-14E9E7B04708}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="1028700"/>
+          <a:ext cx="2200275" cy="2057400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Duper ROM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- fifo status reg</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- fifo read reg</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- fifo write reg</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="正方形/長方形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF7232F4-E500-43DD-A84A-0CD5E1976F64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6000750" y="2400300"/>
+          <a:ext cx="1400175" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>I2C</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Slave</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="正方形/長方形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA2C098-97DA-42DE-B1C8-C5EEB1E7D9A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6000750" y="1028700"/>
+          <a:ext cx="1400175" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>FIFO IN</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE53571D-D08A-4208-A789-A7E9DE084E02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6000750" y="1714500"/>
+          <a:ext cx="1400175" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>FIFO OUT</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A3C8D36-9973-45F2-947C-AFD9F613B0E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="2228850"/>
+          <a:ext cx="1400175" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>PRGROM</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="直線コネクタ 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4573CB36-553A-4896-9393-D4D1F8EB78D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4600575" y="1285875"/>
+          <a:ext cx="1400175" cy="85725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直線コネクタ 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37EE5112-0BB7-497B-B845-1B5A76EC248E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4600575" y="1371600"/>
+          <a:ext cx="1400175" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直線コネクタ 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{235B674C-8406-4421-86C1-22C3E27A332E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4600575" y="1457325"/>
+          <a:ext cx="1400175" cy="85725"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直線コネクタ 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3686753-0F3D-4780-89E8-32BBD14393D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4600575" y="1714501"/>
+          <a:ext cx="1400175" cy="171449"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="正方形/長方形 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F72910D1-106A-48F3-9336-46056147D7C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10201275" y="1314450"/>
+          <a:ext cx="638175" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>GPIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直線コネクタ 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D464D33-B14E-4B55-9B1B-DE556B0FBB96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+          <a:endCxn id="22" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7400925" y="1285875"/>
+          <a:ext cx="2800350" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直線コネクタ 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8566BEBE-CE20-4E1D-91A2-AA2DFB64934C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="22" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7400925" y="1514475"/>
+          <a:ext cx="2800350" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="正方形/長方形 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C0F5110-16E5-4762-9032-73D1CCC95069}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10201275" y="2000250"/>
+          <a:ext cx="638175" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>I2C Master</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="直線コネクタ 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC82FDF8-D793-4A32-BC15-BEE240655175}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="29" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7400925" y="2286000"/>
+          <a:ext cx="2800350" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="正方形/長方形 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2544D606-B49D-46F3-898B-3B4C8E08C8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1200150" y="1200150"/>
+          <a:ext cx="600075" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>CPU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="正方形/長方形 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F1ECFD-B4CE-47A1-9EF8-0B149F2B7120}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1200150" y="1714500"/>
+          <a:ext cx="600075" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>PPU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="直線コネクタ 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{840AA9AC-88C6-4C07-80B0-4035C76069D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="3"/>
+          <a:endCxn id="7" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1800225" y="1371600"/>
+          <a:ext cx="1800225" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="直線コネクタ 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD17308-82AC-48FF-BE04-FFDA927110D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1800225" y="1885950"/>
+          <a:ext cx="1600200" cy="2143125"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4817,7 +6247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -5134,4 +6564,20 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB27B8FE-7E65-4D10-B775-6603DAD80D23}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB37" sqref="AB37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modelsim dev env, rom integration ok.
</commit_message>
<xml_diff>
--- a/doc/super-duper-nes-architecture.xlsx
+++ b/doc/super-duper-nes-architecture.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="architecture" sheetId="1" r:id="rId1"/>
     <sheet name="block diagram" sheetId="2" r:id="rId2"/>
     <sheet name="memory map" sheetId="3" r:id="rId3"/>
     <sheet name="nes-bbb-if" sheetId="4" r:id="rId4"/>
+    <sheet name="fpga-rtl" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Fami con cartlidge I/F</t>
   </si>
@@ -228,6 +229,50 @@
   </si>
   <si>
     <t>always 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/empty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/full</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/data</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/addr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/scl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/sda</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/gpio</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/i2c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/i2c_data_in</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/i2c_data_out</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/composite</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5904,6 +5949,1663 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>74</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="正方形/長方形 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7340808D-B02E-4ADA-A3D2-12C114518764}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18440400" y="3429000"/>
+          <a:ext cx="2095500" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>AM3359</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="正方形/長方形 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5B41102-BD15-4B8D-A8FE-56F95518384D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11106150" y="342900"/>
+          <a:ext cx="7962900" cy="5657850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>de0-cv</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE56944-E785-422E-AC0B-330F7732DF15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="685800"/>
+          <a:ext cx="1257300" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>prgrom</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD54228A-90DD-4B55-95DD-792104F01CAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11734800" y="3943350"/>
+          <a:ext cx="1257300" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>chrrom</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直線コネクタ 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B6A153-AB83-4B25-816A-4BA191604DFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12363450" y="4800600"/>
+          <a:ext cx="0" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直線コネクタ 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F322D273-1E8E-483E-86D0-2616452A6613}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="1543050"/>
+          <a:ext cx="0" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="正方形/長方形 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A3DD3E-9A9A-4A89-B0AD-A1E844E05679}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="2571750"/>
+          <a:ext cx="1257300" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>i2c_slave</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直線コネクタ 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88841D87-5E7B-4ECB-9F4D-160B4FCAB580}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="18" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3771900" y="2057400"/>
+          <a:ext cx="0" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="正方形/長方形 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F82768FD-B4F3-4B94-B639-4C850B9B5A82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5029200" y="2571750"/>
+          <a:ext cx="1257300" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>fifo_in</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直線コネクタ 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D13BA419-B17D-4C57-8E2B-43B95013F224}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="22" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5657850" y="2057400"/>
+          <a:ext cx="0" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="正方形/長方形 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14CE2C1-A8DA-4C29-AEF4-DC1113ED3448}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6915150" y="2571750"/>
+          <a:ext cx="1257300" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>fifo_out</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直線コネクタ 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3FF3C7D-B8B3-4B30-95C8-33683BA16A80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="24" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7543800" y="2057400"/>
+          <a:ext cx="0" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直線コネクタ 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8164CB4-C0A6-45B5-83A0-1F4FC860F3E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="22" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5657850" y="3429000"/>
+          <a:ext cx="0" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直線コネクタ 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44966D97-8850-48B1-BAD3-74C85954AB25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="24" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7543800" y="3429000"/>
+          <a:ext cx="0" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="直線コネクタ 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A67B8748-7FEA-4E93-A811-8DEE3F2E3BED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="18" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3771900" y="3429000"/>
+          <a:ext cx="0" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>76</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="正方形/長方形 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB7F798-3D4B-423A-B024-48F08C5D4698}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18230850" y="3086100"/>
+          <a:ext cx="2095500" cy="1885950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>bbb</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="正方形/長方形 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B7E65A-9681-4E3A-8D86-C3F668682A36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18421350" y="4286250"/>
+          <a:ext cx="857250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>i2c_master</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="直線コネクタ 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01FCFE90-26F7-4121-B994-90BD062BB74B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="42" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12153900" y="4457700"/>
+          <a:ext cx="6267450" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="正方形/長方形 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23BAFA1-E226-45A0-BA91-C111B7B78FF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20535900" y="3771900"/>
+          <a:ext cx="628650" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>gpio</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直線コネクタ 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B153635-017C-4323-BA05-1C1CC64D68B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="48" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15716250" y="3943350"/>
+          <a:ext cx="4819650" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="正方形/長方形 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B3F18D6-BDFC-4820-A255-89D3659CC2C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="1371600"/>
+          <a:ext cx="1676400" cy="4629150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>nes</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="正方形/長方形 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D163874-8179-432D-9A37-EBDAEAA05FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="1714500"/>
+          <a:ext cx="1257300" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>cpu</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="正方形/長方形 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AF5B67D-59A5-406C-8121-AE56AFD3A597}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="4972050"/>
+          <a:ext cx="1257300" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>ppu</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線コネクタ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82AB4AAA-FC9A-4804-B621-BC81E1FC75D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="56" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9848850" y="2057400"/>
+          <a:ext cx="8801100" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直線コネクタ 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55EB6B21-CFFE-4002-A0A6-2A9BC85985B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="58" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9848850" y="5314950"/>
+          <a:ext cx="4191000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="直線コネクタ 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2D73108-23E7-4C47-95B7-E9CC28F77833}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="56" idx="2"/>
+          <a:endCxn id="58" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9220200" y="2400300"/>
+          <a:ext cx="0" cy="2571750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="正方形/長方形 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{264658E5-CF3A-4035-8D4E-8E0B93CE422C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="4972050"/>
+          <a:ext cx="1257300" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>tv</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="直線コネクタ 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DEC997-0EE5-4E83-AB34-EB62764DC302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="3"/>
+          <a:endCxn id="58" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="5314950"/>
+          <a:ext cx="1257300" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6215,7 +7917,7 @@
   <dimension ref="L17:AB18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6570,8 +8272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB27B8FE-7E65-4D10-B775-6603DAD80D23}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB37" sqref="AB37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6580,4 +8282,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42FBB49-54EB-467B-B773-562DC57E2882}">
+  <dimension ref="J11:BM32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="11" spans="27:57" x14ac:dyDescent="0.15">
+      <c r="AA11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="27:57" x14ac:dyDescent="0.15">
+      <c r="AA12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="27:57" x14ac:dyDescent="0.15">
+      <c r="AM13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="27:57" x14ac:dyDescent="0.15">
+      <c r="AM14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="AM21" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="AM22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="BM23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="BM26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="AA30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="AA31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="10:65" x14ac:dyDescent="0.15">
+      <c r="J32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fifo state machine working.
</commit_message>
<xml_diff>
--- a/doc/super-duper-nes-architecture.xlsx
+++ b/doc/super-duper-nes-architecture.xlsx
@@ -8459,13 +8459,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
+      <xdr:col>64</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
+      <xdr:col>68</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -8483,7 +8483,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12144375" y="4114800"/>
+          <a:off x="15240000" y="4114800"/>
           <a:ext cx="952500" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -8708,15 +8708,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>98634</xdr:colOff>
+      <xdr:colOff>98635</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>75326</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>139489</xdr:colOff>
+      <xdr:rowOff>75325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>139490</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>100434</xdr:rowOff>
+      <xdr:rowOff>100433</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8734,12 +8734,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="9155258" y="1086627"/>
-          <a:ext cx="25108" cy="6232105"/>
+          <a:off x="10703071" y="-461186"/>
+          <a:ext cx="25108" cy="9327730"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -4359176"/>
+            <a:gd name="adj1" fmla="val -3714254"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -8863,7 +8863,7 @@
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 564963"/>
+            <a:gd name="adj1" fmla="val 392114"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -8899,7 +8899,7 @@
       <xdr:rowOff>96125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
+      <xdr:col>55</xdr:col>
       <xdr:colOff>139489</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>71017</xdr:rowOff>
@@ -8915,17 +8915,17 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="10" idx="5"/>
-          <a:endCxn id="16" idx="3"/>
+          <a:endCxn id="30" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="8380266" y="2225318"/>
-          <a:ext cx="146342" cy="4803355"/>
+          <a:off x="9570891" y="1034693"/>
+          <a:ext cx="146342" cy="7184605"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 643765"/>
+            <a:gd name="adj1" fmla="val 324838"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -8956,13 +8956,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>98634</xdr:colOff>
+      <xdr:colOff>98635</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>96125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>139489</xdr:colOff>
+      <xdr:col>74</xdr:col>
+      <xdr:colOff>139490</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>71017</xdr:rowOff>
     </xdr:to>
@@ -8977,17 +8977,17 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="10" idx="5"/>
-          <a:endCxn id="17" idx="3"/>
+          <a:endCxn id="44" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="9094641" y="1510943"/>
-          <a:ext cx="146342" cy="6232105"/>
+          <a:off x="11833079" y="-1227494"/>
+          <a:ext cx="146342" cy="11708980"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 871571"/>
+            <a:gd name="adj1" fmla="val 630748"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -9017,13 +9017,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
+      <xdr:col>64</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
+      <xdr:col>68</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -9041,7 +9041,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12144375" y="6343650"/>
+          <a:off x="15240000" y="6343650"/>
           <a:ext cx="952500" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -9207,13 +9207,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>53</xdr:col>
+      <xdr:col>66</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>53</xdr:col>
+      <xdr:col>66</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -9234,7 +9234,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12620625" y="4800600"/>
+          <a:off x="15716250" y="4800600"/>
           <a:ext cx="0" cy="1543050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -9242,6 +9242,622 @@
         </a:prstGeom>
         <a:ln>
           <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="楕円 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5553E96-8785-41AE-9C67-BF2FDD0FFD26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11906250" y="4114800"/>
+          <a:ext cx="952500" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>fifo pop</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="楕円 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA2EFB9C-B4D2-4697-90A8-A4FD4B79FED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13096875" y="4114800"/>
+          <a:ext cx="952500" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>fifo read ok</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>104984</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>94084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>145839</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106784</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="コネクタ: 曲線 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E94192-955E-4141-9A1E-7BCB8A922426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="16" idx="7"/>
+          <a:endCxn id="29" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="11787187" y="3956681"/>
+          <a:ext cx="12700" cy="517105"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2590811"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>104984</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>94084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>145839</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106784</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="コネクタ: 曲線 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{501E4B56-0819-4FD1-9ACC-1599D0F51507}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="29" idx="7"/>
+          <a:endCxn id="30" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="12977812" y="3956681"/>
+          <a:ext cx="12700" cy="517105"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2590811"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>92285</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106783</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>104985</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>77367</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="コネクタ: 曲線 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81C018E2-ADED-44C0-AF56-563DABE33CF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="30" idx="7"/>
+          <a:endCxn id="30" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="13667418" y="4457700"/>
+          <a:ext cx="484934" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -47140"/>
+            <a:gd name="adj2" fmla="val 8201654"/>
+            <a:gd name="adj3" fmla="val 147140"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="楕円 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64B4E926-0762-4832-800A-D5F663D11DA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16430625" y="4114800"/>
+          <a:ext cx="952500" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>fifo push</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>74</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="楕円 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794AD72E-7D1C-4101-8957-74F96AEB3147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17621250" y="4114800"/>
+          <a:ext cx="952500" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>fifo write ok</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>104984</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>94084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>145839</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106784</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="コネクタ: 曲線 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{468D0F7F-35BA-4071-8DB1-E9A87F05AC70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="17" idx="7"/>
+          <a:endCxn id="43" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="16311562" y="3956681"/>
+          <a:ext cx="12700" cy="517105"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2590811"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>104984</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>94084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>74</xdr:col>
+      <xdr:colOff>145839</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106784</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="コネクタ: 曲線 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE2B56E2-BE96-480C-A1F7-94DC556582E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="43" idx="7"/>
+          <a:endCxn id="44" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="17502187" y="3956681"/>
+          <a:ext cx="12700" cy="517105"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2590811"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>92285</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106783</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>104985</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>77367</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="コネクタ: 曲線 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E384624-0762-4127-A63B-4DE9E4272DA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="7"/>
+          <a:endCxn id="44" idx="5"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="18191793" y="4457700"/>
+          <a:ext cx="484934" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -47140"/>
+            <a:gd name="adj2" fmla="val 8201654"/>
+            <a:gd name="adj3" fmla="val 147140"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -10031,8 +10647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88CBFEC-A20F-44E2-9A89-ADFAF373EA5B}">
   <dimension ref="H5:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY34" sqref="AY34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
nes push fifo oookey.
</commit_message>
<xml_diff>
--- a/doc/super-duper-nes-architecture.xlsx
+++ b/doc/super-duper-nes-architecture.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="141">
   <si>
     <t>Fami con cartlidge I/F</t>
   </si>
@@ -551,6 +551,26 @@
   <si>
     <t>Address = 0x44 ( 100 0100)</t>
   </si>
+  <si>
+    <t>idle</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rom</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>i2c xfer</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>i2c ack</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>i2c idle</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
@@ -611,7 +631,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,6 +653,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,7 +788,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -794,6 +832,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -24377,6 +24421,66 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>77875</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>21841</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>138254</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>144069</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="495" name="矢印: 上 494">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC96DBAB-5DAE-4DDD-AFE6-E6B01DD7F3F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8812120" y="13509600"/>
+          <a:ext cx="60379" cy="805153"/>
+        </a:xfrm>
+        <a:prstGeom prst="upArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -30409,10 +30513,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88CBFEC-A20F-44E2-9A89-ADFAF373EA5B}">
-  <dimension ref="F5:BP69"/>
+  <dimension ref="F5:BP85"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="AK46" sqref="AK46"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="AN82" sqref="AN82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
@@ -30570,13 +30674,200 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="14:45">
+    <row r="69" spans="14:53">
       <c r="N69" t="s">
         <v>113</v>
       </c>
       <c r="AS69" t="s">
         <v>114</v>
       </c>
+    </row>
+    <row r="79" spans="14:53">
+      <c r="N79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="O79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="P79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="R79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="S79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="T79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="U79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="V79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="W79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="X79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AV79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AX79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY79" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ79" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA79" s="26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="14:53" s="28" customFormat="1"/>
+    <row r="81" spans="6:58" s="28" customFormat="1"/>
+    <row r="82" spans="6:58" s="28" customFormat="1"/>
+    <row r="83" spans="6:58" s="28" customFormat="1"/>
+    <row r="85" spans="6:58">
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="23"/>
+      <c r="J85" s="23"/>
+      <c r="K85" s="23"/>
+      <c r="L85" s="23"/>
+      <c r="M85" s="23"/>
+      <c r="N85" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="O85" s="23"/>
+      <c r="P85" s="23"/>
+      <c r="Q85" s="23"/>
+      <c r="R85" s="23"/>
+      <c r="S85" s="23"/>
+      <c r="T85" s="23"/>
+      <c r="U85" s="23"/>
+      <c r="V85" s="23"/>
+      <c r="W85" s="23"/>
+      <c r="X85" s="23"/>
+      <c r="Y85" s="23"/>
+      <c r="Z85" s="23"/>
+      <c r="AA85" s="23"/>
+      <c r="AB85" s="23"/>
+      <c r="AC85" s="23"/>
+      <c r="AD85" s="23"/>
+      <c r="AE85" s="23"/>
+      <c r="AF85" s="23"/>
+      <c r="AG85" s="23"/>
+      <c r="AH85" s="23"/>
+      <c r="AI85" s="23"/>
+      <c r="AJ85" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK85" s="25"/>
+      <c r="AL85" s="25"/>
+      <c r="AM85" s="25"/>
+      <c r="AN85" s="25"/>
+      <c r="AO85" s="25"/>
+      <c r="AP85" s="25"/>
+      <c r="AQ85" s="25"/>
+      <c r="AR85" s="25"/>
+      <c r="AS85" s="25"/>
+      <c r="AT85" s="25"/>
+      <c r="AU85" s="25"/>
+      <c r="AV85" s="25"/>
+      <c r="AW85" s="25"/>
+      <c r="AX85" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY85" s="27"/>
+      <c r="AZ85" s="27"/>
+      <c r="BA85" s="27"/>
+      <c r="BB85" s="27"/>
+      <c r="BC85" s="27"/>
+      <c r="BD85" s="27"/>
+      <c r="BE85" s="27"/>
+      <c r="BF85" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -31274,7 +31565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B437FFD9-859C-40BE-A265-40ADB9507666}">
   <dimension ref="A47:DP82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozenSplit"/>
       <selection activeCell="A31" sqref="A31"/>
       <selection pane="topRight" activeCell="BL37" sqref="BL37"/>
@@ -31439,11 +31730,11 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>